<commit_message>
Forgot to add the files to commit.
</commit_message>
<xml_diff>
--- a/ClosedSections.xlsx
+++ b/ClosedSections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnwob\GitHub\ShearFlowThinSections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF0569E-E4A8-494A-A427-BFF86A07DA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193AB5DB-FBE0-446C-8BD3-F3A5636C3140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="26835" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="5715" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Section </t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Yc</t>
+  </si>
+  <si>
+    <t>Zc</t>
   </si>
 </sst>
 </file>
@@ -352,18 +358,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -371,34 +378,66 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0.25</v>
+      </c>
+      <c r="C2">
+        <v>0.125</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.25</v>
+      </c>
+      <c r="C3">
+        <v>-0.125</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="F3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="1"/>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Shear Center Reference point added
The shear center reference point must now be added for all sections. The shear center will be calculated with respect to this point.
</commit_message>
<xml_diff>
--- a/ClosedSections.xlsx
+++ b/ClosedSections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnwob\GitHub\ShearFlowThinSections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnwob\GitHub\ShearFlowThinSections\tests\ex2_open_section\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193AB5DB-FBE0-446C-8BD3-F3A5636C3140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2BC8BF-13A1-4368-A374-8CBB517DADD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="5715" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="5025" windowWidth="26835" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Section </t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>Yc</t>
-  </si>
-  <si>
-    <t>Zc</t>
   </si>
 </sst>
 </file>
@@ -361,13 +355,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -378,66 +371,37 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.125</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0.25</v>
-      </c>
-      <c r="C2">
-        <v>0.125</v>
-      </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.25</v>
-      </c>
-      <c r="C3">
-        <v>-0.125</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1">
-        <v>8</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>